<commit_message>
adding nutrient data from sessions 53 west and 28-29 south along with new 2019 1st quarter web exports that do not include insitu only samples
</commit_message>
<xml_diff>
--- a/db/reports/web-export-starting-file.xlsx
+++ b/db/reports/web-export-starting-file.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="46360" windowHeight="26720" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meta data" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -72,9 +72,6 @@
     <t>Data with #N/A have been quality assured and the value did not meet the parameter guidelines due to problems with calibration, verification, sampling or analysis. Further information on these missing values can be made available on request.</t>
   </si>
   <si>
-    <t>Falinski, Kim, Reed, Dana, Callender, Tova, Fielding, Emily, Newbold, Robin, &amp; Yurkanin, Alana. (2017). Hui o ka Wai Ola Water Quality Data [Data set]. Zenodo. http://doi.org/10.5281/zenodo.830050</t>
-  </si>
-  <si>
     <t>Parameter Type</t>
   </si>
   <si>
@@ -173,19 +170,16 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Falinski, Kim, Reed, Dana, Callender, Tova, Fielding, Emily, Newbold, Robin, &amp; Yurkanin, Alana. (2017). Hui o ka Wai Ola Water Quality Data [Data set]. Zenodo. http://doi.org/10.5281/zenodo.830049</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -252,7 +246,7 @@
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -575,14 +569,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D26"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="2" max="2" width="42.42578125" customWidth="1"/>
@@ -621,7 +615,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -636,38 +630,38 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" ht="14">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" ht="14">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -677,13 +671,13 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="14">
@@ -691,13 +685,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="14">
@@ -705,13 +699,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="14">
@@ -719,13 +713,13 @@
         <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="14">
@@ -733,13 +727,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="14">
@@ -747,13 +741,13 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28">
@@ -761,13 +755,13 @@
         <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="28">
@@ -775,13 +769,13 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28">
@@ -789,13 +783,13 @@
         <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="28">
@@ -803,13 +797,13 @@
         <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="28">
@@ -817,13 +811,13 @@
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="28">
@@ -831,13 +825,13 @@
         <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14">
@@ -849,7 +843,7 @@
     <row r="23" spans="1:4" ht="14" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -877,7 +871,6 @@
       <c r="D26" s="5"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B25:D26"/>
@@ -885,7 +878,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>